<commit_message>
Correção em relação aos resumos dos capitulos 2, 3, 4 e 5
</commit_message>
<xml_diff>
--- a/figuras/Coverage.xlsx
+++ b/figuras/Coverage.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Angel\Desktop\Dissertacao_QtOm\figuras\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="860" yWindow="2780" windowWidth="35120" windowHeight="23320" tabRatio="500"/>
+    <workbookView xWindow="855" yWindow="2775" windowWidth="35115" windowHeight="23325" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -305,6 +310,14 @@
       <color rgb="FF00C802"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -330,8 +343,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.103448288433792"/>
-          <c:y val="0.012"/>
-          <c:w val="0.815128245559188"/>
+          <c:y val="1.2E-2"/>
+          <c:w val="0.81512824555918795"/>
           <c:h val="0.928672309711286"/>
         </c:manualLayout>
       </c:layout>
@@ -430,34 +443,34 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.9066</c:v>
+                  <c:v>0.90659999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8181</c:v>
+                  <c:v>0.81810000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.915</c:v>
+                  <c:v>0.91500000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.8881</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.908</c:v>
+                  <c:v>0.90800000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8709</c:v>
+                  <c:v>0.87090000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.8333</c:v>
+                  <c:v>0.83330000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,31 +572,31 @@
                   <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8787</c:v>
+                  <c:v>0.87870000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8936</c:v>
+                  <c:v>0.89359999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.6781</c:v>
+                  <c:v>0.67810000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.6774</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,31 +698,31 @@
                   <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.8484</c:v>
+                  <c:v>0.84840000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.8617</c:v>
+                  <c:v>0.86170000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.921</c:v>
+                  <c:v>0.92100000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.8275</c:v>
+                  <c:v>0.82750000000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.8709</c:v>
+                  <c:v>0.87090000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,16 +739,17 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134842536"/>
-        <c:axId val="2134834712"/>
+        <c:axId val="-1245550736"/>
+        <c:axId val="-1245547472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134842536"/>
+        <c:axId val="-1245550736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -749,10 +763,10 @@
                 <a:cs typeface="Palatino Linotype"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134834712"/>
+        <c:crossAx val="-1245547472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -760,11 +774,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2134834712"/>
+        <c:axId val="-1245547472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -787,10 +801,10 @@
                 <a:cs typeface="Palatino Linotype"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2134842536"/>
+        <c:crossAx val="-1245550736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -802,10 +816,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.911631285700354"/>
-          <c:y val="0.419942125984252"/>
-          <c:w val="0.0883687142996464"/>
-          <c:h val="0.120115748031496"/>
+          <c:x val="0.91163128570035401"/>
+          <c:y val="0.41994212598425201"/>
+          <c:w val="8.8368714299646406E-2"/>
+          <c:h val="0.12011574803149599"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -819,7 +833,7 @@
               <a:cs typeface="Palatino Linotype"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="pt-BR"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -834,7 +848,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1201,13 +1215,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">

</xml_diff>

<commit_message>
Correções das figuras presente na dissertação
</commit_message>
<xml_diff>
--- a/figuras/Coverage.xlsx
+++ b/figuras/Coverage.xlsx
@@ -65,10 +65,10 @@
     <t>DIVINE</t>
   </si>
   <si>
-    <t>Associative Containers</t>
+    <t>Containers Associativos</t>
   </si>
   <si>
-    <t>Sequential Containers</t>
+    <t>Containers Sequenciais</t>
   </si>
 </sst>
 </file>
@@ -427,10 +427,10 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Associative Containers</c:v>
+                    <c:v>Containers Associativos</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Sequential Containers</c:v>
+                    <c:v>Containers Sequenciais</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -553,10 +553,10 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Associative Containers</c:v>
+                    <c:v>Containers Associativos</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Sequential Containers</c:v>
+                    <c:v>Containers Sequenciais</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -679,10 +679,10 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Associative Containers</c:v>
+                    <c:v>Containers Associativos</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Sequential Containers</c:v>
+                    <c:v>Containers Sequenciais</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -739,11 +739,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1245550736"/>
-        <c:axId val="-1245547472"/>
+        <c:axId val="1558896816"/>
+        <c:axId val="1558893552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1245550736"/>
+        <c:axId val="1558896816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,7 +766,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1245547472"/>
+        <c:crossAx val="1558893552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -774,7 +774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1245547472"/>
+        <c:axId val="1558893552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -804,7 +804,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1245550736"/>
+        <c:crossAx val="1558896816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="0.2"/>
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>